<commit_message>
winners image added and some minor UI changes
</commit_message>
<xml_diff>
--- a/gifts.xlsx
+++ b/gifts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ballot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\roots-tech-lucky-draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF3E240-6B41-4516-BD69-71C43F67748A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9D78C7-7917-4402-92CD-4CE797E37C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2C1416CA-A29A-43E3-BC91-6D1420C2E0CF}"/>
   </bookViews>
@@ -25,89 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
-  <si>
-    <t>Audionic speaker Sugar 20</t>
-  </si>
-  <si>
-    <t>l800 speaker</t>
-  </si>
-  <si>
-    <t>Audionic headphones</t>
-  </si>
-  <si>
-    <t>audionic solo x9</t>
-  </si>
-  <si>
-    <t>ronin power banks</t>
-  </si>
-  <si>
-    <t>mi airdots</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 21</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 22</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 23</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 24</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 25</t>
-  </si>
-  <si>
-    <t>Audionic speaker Sugar 26</t>
-  </si>
-  <si>
-    <t>Ronin headphones</t>
-  </si>
-  <si>
-    <t>audionic solo x10</t>
-  </si>
-  <si>
-    <t>audionic solo x11</t>
-  </si>
-  <si>
-    <t>Ronin Chargers</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
   <si>
     <t>Smart Watch</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Android </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ox</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Audionic Speaker G5 </t>
   </si>
   <si>
     <t>Gifts</t>
+  </si>
+  <si>
+    <t>Audionic Speaker Sugar 20</t>
+  </si>
+  <si>
+    <t>L800 speaker</t>
+  </si>
+  <si>
+    <t>Audionic solo x9</t>
+  </si>
+  <si>
+    <t>Audionic Bluetooth Headphone</t>
+  </si>
+  <si>
+    <t>Ronin Wireless Headphone</t>
+  </si>
+  <si>
+    <t>Android Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ronin Power Bank </t>
+  </si>
+  <si>
+    <t>Mi Airdot</t>
+  </si>
+  <si>
+    <t>Ronin Charger</t>
   </si>
 </sst>
 </file>
@@ -492,285 +445,286 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBFD2F6-3D83-48A6-BDEC-678F1E2D9EFF}">
   <dimension ref="A1:A54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>